<commit_message>
resource data and such
</commit_message>
<xml_diff>
--- a/shinyapp/data/Health and Social Services.xlsx
+++ b/shinyapp/data/Health and Social Services.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209032AB-4EA2-8B42-8D77-03D2933E0DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84385E20-1B59-5142-A463-BC5B0EE59F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{C2343199-C9B2-344C-BAE9-B0A04F918DEC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="2" xr2:uid="{C2343199-C9B2-344C-BAE9-B0A04F918DEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Food" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>Latitude</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t xml:space="preserve">Location </t>
-  </si>
-  <si>
-    <t>Organization name</t>
   </si>
   <si>
     <t>Loudoun Hunger Relief</t>
@@ -113,7 +110,19 @@
     <t>VisionWorks</t>
   </si>
   <si>
-    <t>,-77.4132603</t>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>Food</t>
   </si>
 </sst>
 </file>
@@ -487,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3827FC-CA28-3749-8E33-05EE47793579}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,7 +509,7 @@
     <col min="3" max="3" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -510,10 +519,13 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>39.082056299999998</v>
@@ -521,10 +533,13 @@
       <c r="C2">
         <v>-77.555456000000007</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>38.977684000000004</v>
@@ -532,10 +547,13 @@
       <c r="C3">
         <v>-77.424610000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>38.952911800000003</v>
@@ -543,10 +561,13 @@
       <c r="C4">
         <v>-77.349882899999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>39.033757299999998</v>
@@ -554,10 +575,13 @@
       <c r="C5">
         <v>-77.517221800000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>39.118936400000003</v>
@@ -565,10 +589,13 @@
       <c r="C6">
         <v>-77.549949100000006</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>38.905459999999998</v>
@@ -576,10 +603,13 @@
       <c r="C7">
         <v>-77.528904999999995</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>39.1393269</v>
@@ -587,10 +617,13 @@
       <c r="C8">
         <v>-77.715578399999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>39.109718000000001</v>
@@ -598,8 +631,11 @@
       <c r="C9">
         <v>-77.556811499999995</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
     </row>
   </sheetData>
@@ -609,10 +645,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD409E3-F850-CF4B-A17F-855938358841}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,9 +658,9 @@
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -632,10 +668,13 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>38.992925700000001</v>
@@ -643,10 +682,13 @@
       <c r="C2">
         <v>-77.426618700000006</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>38.913342999999998</v>
@@ -654,10 +696,13 @@
       <c r="C3">
         <v>-77.511601999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>39.100707700000001</v>
@@ -665,10 +710,13 @@
       <c r="C4">
         <v>-77.539245800000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
         <v>38.948372599999999</v>
@@ -676,10 +724,13 @@
       <c r="C5">
         <v>-77.330610800000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>39.0143536</v>
@@ -687,10 +738,13 @@
       <c r="C6">
         <v>-77.375699499999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>39.137821000000002</v>
@@ -698,8 +752,11 @@
       <c r="C7">
         <v>-77.715688</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
     </row>
   </sheetData>
@@ -709,10 +766,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146EB6B2-89E2-754F-9E73-797E47276B55}">
-  <dimension ref="A1:C1001"/>
+  <dimension ref="A1:D1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,9 +778,9 @@
     <col min="2" max="2" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -731,10 +788,13 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>38.964375400000002</v>
@@ -742,10 +802,13 @@
       <c r="C2">
         <v>-77.397841900000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>39.024825700000001</v>
@@ -753,10 +816,13 @@
       <c r="C3">
         <v>-77.3927944</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>39.116802200000002</v>
@@ -764,10 +830,13 @@
       <c r="C4">
         <v>-77.564622499999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>39.113897999999999</v>
@@ -775,10 +844,13 @@
       <c r="C5">
         <v>-77.561629999999994</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>39.023046999999998</v>
@@ -786,21 +858,27 @@
       <c r="C6">
         <v>-77.399366999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
         <v>39.037760200000001</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>-77.413260300000005</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
         <v>39.0323712</v>
@@ -808,10 +886,13 @@
       <c r="C8">
         <v>-77.423812299999994</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1">
         <v>38.935834999999997</v>
@@ -819,26 +900,29 @@
       <c r="C9">
         <v>-77.331604999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>